<commit_message>
Identification request and response encoding and decoding
</commit_message>
<xml_diff>
--- a/scripts/GtpV2StackCodeGen/dataModel/prototypeV8.xlsx
+++ b/scripts/GtpV2StackCodeGen/dataModel/prototypeV8.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Message Modeling" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4684" uniqueCount="1564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4680" uniqueCount="1564">
   <si>
     <t xml:space="preserve">Message Definition Start:CreateSessionRequest:32</t>
   </si>
@@ -3706,10 +3706,6 @@
 "Request accepted". </t>
   </si>
   <si>
-    <t xml:space="preserve">This IE shall be included when session trace is active for
-this IMSI/IMEI. </t>
-  </si>
-  <si>
     <t xml:space="preserve">UE Usage Type </t>
   </si>
   <si>
@@ -3798,6 +3794,10 @@
   </si>
   <si>
     <t xml:space="preserve">Trace Information </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This IE shall be included when session trace is active for
+this IMSI/IMEI. </t>
   </si>
   <si>
     <t xml:space="preserve">This IE is optionally sent by the MME/S4-SGSN to the peer
@@ -8293,8 +8293,8 @@
   </sheetPr>
   <dimension ref="B2:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B835" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B840" activeCellId="0" sqref="B840"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B843" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A847" activeCellId="0" sqref="A847"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19856,7 +19856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="840" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B840" s="26" t="s">
         <v>604</v>
       </c>
@@ -19938,156 +19938,156 @@
         <v>0</v>
       </c>
     </row>
-    <row r="847" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="847" customFormat="false" ht="240.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B847" s="18"/>
       <c r="C847" s="18"/>
       <c r="D847" s="7" t="s">
-        <v>83</v>
+        <v>608</v>
       </c>
       <c r="E847" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F847" s="9" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="G847" s="11" t="s">
-        <v>83</v>
+        <v>156</v>
       </c>
       <c r="H847" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="848" customFormat="false" ht="240.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="848" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B848" s="18"/>
       <c r="C848" s="18"/>
       <c r="D848" s="7" t="s">
-        <v>609</v>
+        <v>580</v>
       </c>
       <c r="E848" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F848" s="9" t="s">
+        <v>581</v>
+      </c>
+      <c r="F848" s="9"/>
+      <c r="G848" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="H848" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B849" s="26" t="s">
         <v>610</v>
       </c>
-      <c r="G848" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="H848" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="849" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B849" s="18"/>
-      <c r="C849" s="18"/>
-      <c r="D849" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="E849" s="7" t="s">
-        <v>581</v>
-      </c>
-      <c r="F849" s="9"/>
-      <c r="G849" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="H849" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="850" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B850" s="26" t="s">
+      <c r="C849" s="26"/>
+      <c r="D849" s="26"/>
+      <c r="E849" s="26"/>
+      <c r="F849" s="26"/>
+      <c r="G849" s="26"/>
+      <c r="H849" s="26"/>
+    </row>
+    <row r="851" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B852" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="C850" s="26"/>
-      <c r="D850" s="26"/>
-      <c r="E850" s="26"/>
-      <c r="F850" s="26"/>
-      <c r="G850" s="26"/>
-      <c r="H850" s="26"/>
-    </row>
-    <row r="852" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C852" s="1"/>
+      <c r="D852" s="1"/>
+      <c r="E852" s="1"/>
+      <c r="F852" s="1"/>
+      <c r="G852" s="1"/>
+      <c r="H852" s="1"/>
+    </row>
     <row r="853" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B853" s="1" t="s">
+      <c r="B853" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C853" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D853" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E853" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F853" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G853" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H853" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="854" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B854" s="18"/>
+      <c r="C854" s="18"/>
+      <c r="D854" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="E854" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="F854" s="9" t="s">
         <v>612</v>
       </c>
-      <c r="C853" s="1"/>
-      <c r="D853" s="1"/>
-      <c r="E853" s="1"/>
-      <c r="F853" s="1"/>
-      <c r="G853" s="1"/>
-      <c r="H853" s="1"/>
-    </row>
-    <row r="854" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B854" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C854" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D854" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E854" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F854" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G854" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H854" s="4" t="s">
-        <v>7</v>
+      <c r="G854" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="H854" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="855" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B855" s="18"/>
       <c r="C855" s="18"/>
       <c r="D855" s="7" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="E855" s="7" t="s">
-        <v>566</v>
+        <v>9</v>
       </c>
       <c r="F855" s="9" t="s">
         <v>613</v>
       </c>
       <c r="G855" s="11" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="H855" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="856" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="856" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B856" s="18"/>
       <c r="C856" s="18"/>
-      <c r="D856" s="7" t="s">
-        <v>600</v>
+      <c r="D856" s="11" t="s">
+        <v>614</v>
       </c>
       <c r="E856" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F856" s="9" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="G856" s="11" t="s">
-        <v>600</v>
+        <v>616</v>
       </c>
       <c r="H856" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="857" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="857" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B857" s="18"/>
       <c r="C857" s="18"/>
-      <c r="D857" s="11" t="s">
-        <v>615</v>
+      <c r="D857" s="7" t="s">
+        <v>617</v>
       </c>
       <c r="E857" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F857" s="9" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="G857" s="11" t="s">
         <v>617</v>
@@ -20096,287 +20096,269 @@
         <v>0</v>
       </c>
     </row>
-    <row r="858" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="858" customFormat="false" ht="150.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B858" s="18"/>
       <c r="C858" s="18"/>
       <c r="D858" s="7" t="s">
-        <v>618</v>
+        <v>587</v>
       </c>
       <c r="E858" s="7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F858" s="9" t="s">
         <v>619</v>
       </c>
       <c r="G858" s="11" t="s">
-        <v>618</v>
+        <v>587</v>
       </c>
       <c r="H858" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="859" customFormat="false" ht="150.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="859" customFormat="false" ht="105.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B859" s="18"/>
       <c r="C859" s="18"/>
       <c r="D859" s="7" t="s">
-        <v>587</v>
+        <v>620</v>
       </c>
       <c r="E859" s="7" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="F859" s="9" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="G859" s="11" t="s">
-        <v>587</v>
+        <v>108</v>
       </c>
       <c r="H859" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="860" customFormat="false" ht="105.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B860" s="18"/>
-      <c r="C860" s="18"/>
-      <c r="D860" s="7" t="s">
-        <v>621</v>
-      </c>
-      <c r="E860" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F860" s="9" t="s">
+    <row r="860" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B860" s="26" t="s">
         <v>622</v>
       </c>
-      <c r="G860" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="H860" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="861" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B861" s="26" t="s">
+      <c r="C860" s="26"/>
+      <c r="D860" s="26"/>
+      <c r="E860" s="26"/>
+      <c r="F860" s="26"/>
+      <c r="G860" s="26"/>
+      <c r="H860" s="26"/>
+    </row>
+    <row r="862" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B863" s="1" t="s">
         <v>623</v>
       </c>
-      <c r="C861" s="26"/>
-      <c r="D861" s="26"/>
-      <c r="E861" s="26"/>
-      <c r="F861" s="26"/>
-      <c r="G861" s="26"/>
-      <c r="H861" s="26"/>
-    </row>
-    <row r="863" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C863" s="1"/>
+      <c r="D863" s="1"/>
+      <c r="E863" s="1"/>
+      <c r="F863" s="1"/>
+      <c r="G863" s="1"/>
+      <c r="H863" s="1"/>
+    </row>
     <row r="864" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B864" s="1" t="s">
-        <v>624</v>
-      </c>
-      <c r="C864" s="1"/>
-      <c r="D864" s="1"/>
-      <c r="E864" s="1"/>
-      <c r="F864" s="1"/>
-      <c r="G864" s="1"/>
-      <c r="H864" s="1"/>
+      <c r="B864" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C864" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D864" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E864" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F864" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G864" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H864" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="865" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B865" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C865" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D865" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E865" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F865" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G865" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H865" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="866" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B865" s="18"/>
+      <c r="C865" s="18"/>
+      <c r="D865" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="E865" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F865" s="9"/>
+      <c r="G865" s="11" t="s">
+        <v>579</v>
+      </c>
+      <c r="H865" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="866" customFormat="false" ht="150.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B866" s="18"/>
       <c r="C866" s="18"/>
       <c r="D866" s="7" t="s">
-        <v>579</v>
+        <v>606</v>
       </c>
       <c r="E866" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F866" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="F866" s="9" t="s">
+        <v>624</v>
+      </c>
       <c r="G866" s="11" t="s">
-        <v>579</v>
+        <v>606</v>
       </c>
       <c r="H866" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="867" customFormat="false" ht="150.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="867" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B867" s="18"/>
       <c r="C867" s="18"/>
       <c r="D867" s="7" t="s">
-        <v>606</v>
+        <v>625</v>
       </c>
       <c r="E867" s="7" t="s">
         <v>9</v>
       </c>
       <c r="F867" s="9" t="s">
+        <v>626</v>
+      </c>
+      <c r="G867" s="11" t="s">
         <v>625</v>
       </c>
-      <c r="G867" s="11" t="s">
-        <v>606</v>
-      </c>
       <c r="H867" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="868" customFormat="false" ht="45.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="868" customFormat="false" ht="105.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B868" s="18"/>
       <c r="C868" s="18"/>
       <c r="D868" s="7" t="s">
-        <v>626</v>
+        <v>106</v>
       </c>
       <c r="E868" s="7" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="F868" s="9" t="s">
-        <v>608</v>
+        <v>627</v>
       </c>
       <c r="G868" s="11" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="H868" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="869" customFormat="false" ht="105.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="869" customFormat="false" ht="285.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B869" s="18"/>
       <c r="C869" s="18"/>
       <c r="D869" s="7" t="s">
-        <v>106</v>
+        <v>608</v>
       </c>
       <c r="E869" s="7" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="F869" s="9" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="G869" s="11" t="s">
-        <v>628</v>
+        <v>156</v>
       </c>
       <c r="H869" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="870" customFormat="false" ht="285.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="870" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B870" s="18"/>
       <c r="C870" s="18"/>
       <c r="D870" s="7" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="E870" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F870" s="9" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="G870" s="11" t="s">
-        <v>156</v>
+        <v>617</v>
       </c>
       <c r="H870" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="871" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="871" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B871" s="18"/>
       <c r="C871" s="18"/>
-      <c r="D871" s="7" t="s">
-        <v>618</v>
+      <c r="D871" s="11" t="s">
+        <v>631</v>
       </c>
       <c r="E871" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F871" s="9" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
       <c r="G871" s="11" t="s">
-        <v>618</v>
+        <v>633</v>
       </c>
       <c r="H871" s="7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="872" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="872" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B872" s="18"/>
       <c r="C872" s="18"/>
       <c r="D872" s="11" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="E872" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F872" s="9" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="G872" s="11" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="H872" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="873" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="873" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B873" s="18"/>
       <c r="C873" s="18"/>
-      <c r="D873" s="11" t="s">
-        <v>634</v>
+      <c r="D873" s="7" t="s">
+        <v>580</v>
       </c>
       <c r="E873" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F873" s="9" t="s">
-        <v>635</v>
-      </c>
+        <v>581</v>
+      </c>
+      <c r="F873" s="9"/>
       <c r="G873" s="11" t="s">
-        <v>636</v>
-      </c>
-      <c r="H873" s="7" t="n">
-        <v>1</v>
+        <v>196</v>
+      </c>
+      <c r="H873" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="874" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B874" s="18"/>
-      <c r="C874" s="18"/>
-      <c r="D874" s="7" t="s">
-        <v>580</v>
-      </c>
-      <c r="E874" s="7" t="s">
-        <v>581</v>
-      </c>
-      <c r="F874" s="9"/>
-      <c r="G874" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="H874" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="875" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B875" s="26" t="s">
+      <c r="B874" s="26" t="s">
         <v>637</v>
       </c>
-      <c r="C875" s="26"/>
-      <c r="D875" s="26"/>
-      <c r="E875" s="26"/>
-      <c r="F875" s="26"/>
-      <c r="G875" s="26"/>
-      <c r="H875" s="26"/>
-    </row>
+      <c r="C874" s="26"/>
+      <c r="D874" s="26"/>
+      <c r="E874" s="26"/>
+      <c r="F874" s="26"/>
+      <c r="G874" s="26"/>
+      <c r="H874" s="26"/>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="414">
@@ -20789,11 +20771,11 @@
     <mergeCell ref="B836:H836"/>
     <mergeCell ref="B840:H840"/>
     <mergeCell ref="B843:H843"/>
-    <mergeCell ref="B850:H850"/>
-    <mergeCell ref="B853:H853"/>
-    <mergeCell ref="B861:H861"/>
-    <mergeCell ref="B864:H864"/>
-    <mergeCell ref="B875:H875"/>
+    <mergeCell ref="B849:H849"/>
+    <mergeCell ref="B852:H852"/>
+    <mergeCell ref="B860:H860"/>
+    <mergeCell ref="B863:H863"/>
+    <mergeCell ref="B874:H874"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -20812,7 +20794,7 @@
   </sheetPr>
   <dimension ref="A2:N847"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A805" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A805" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B453" activeCellId="0" sqref="B453"/>
     </sheetView>
   </sheetViews>

</xml_diff>